<commit_message>
fix complete design-pattern for insert classes
</commit_message>
<xml_diff>
--- a/import/List_group.xlsx
+++ b/import/List_group.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\L A P T R I N H V I EN WEBSITE\Cd2\nckh_ng\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C2CD92-E245-41A9-9170-F1AD888C0A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3EFB31-9BD9-4A0F-93D5-4BB85E8E6670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E6A71C13-185B-42A7-A4FA-5B290892829C}"/>
   </bookViews>
@@ -36,22 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="61">
   <si>
     <t>23211TT2984</t>
   </si>
@@ -68,33 +53,6 @@
     <t>TV</t>
   </si>
   <si>
-    <t>23211TT2981</t>
-  </si>
-  <si>
-    <t>23211TT2982</t>
-  </si>
-  <si>
-    <t>23211TT2983</t>
-  </si>
-  <si>
-    <t>23211TT2911</t>
-  </si>
-  <si>
-    <t>23211TT2912</t>
-  </si>
-  <si>
-    <t>23211TT2921</t>
-  </si>
-  <si>
-    <t>23211TT2184</t>
-  </si>
-  <si>
-    <t>23211TT1984</t>
-  </si>
-  <si>
-    <t>23211TT1114</t>
-  </si>
-  <si>
     <t>TEN_NHOM</t>
   </si>
   <si>
@@ -105,6 +63,162 @@
   </si>
   <si>
     <t>SINH_VIEN</t>
+  </si>
+  <si>
+    <t>23211TT3144</t>
+  </si>
+  <si>
+    <t>21211TT3802</t>
+  </si>
+  <si>
+    <t>21211TT4493</t>
+  </si>
+  <si>
+    <t>21211TT4824</t>
+  </si>
+  <si>
+    <t>22211TT2183</t>
+  </si>
+  <si>
+    <t>22211TT3455</t>
+  </si>
+  <si>
+    <t>23211TT0403</t>
+  </si>
+  <si>
+    <t>23211TT0774</t>
+  </si>
+  <si>
+    <t>22211TT2666</t>
+  </si>
+  <si>
+    <t>23211TT4312</t>
+  </si>
+  <si>
+    <t>23211TT0325</t>
+  </si>
+  <si>
+    <t>23211TT3424</t>
+  </si>
+  <si>
+    <t>23211TT1158</t>
+  </si>
+  <si>
+    <t>23211TT0068</t>
+  </si>
+  <si>
+    <t>23211TT0659</t>
+  </si>
+  <si>
+    <t>22211TT3957</t>
+  </si>
+  <si>
+    <t>22211TT4259</t>
+  </si>
+  <si>
+    <t>23211TT0087</t>
+  </si>
+  <si>
+    <t>23211TT2438</t>
+  </si>
+  <si>
+    <t>21211TT1402</t>
+  </si>
+  <si>
+    <t>23211TT4636</t>
+  </si>
+  <si>
+    <t>23211TT4524</t>
+  </si>
+  <si>
+    <t>23211TT4445</t>
+  </si>
+  <si>
+    <t>22211TT3477</t>
+  </si>
+  <si>
+    <t>23211TT0653</t>
+  </si>
+  <si>
+    <t>23211TT0388</t>
+  </si>
+  <si>
+    <t>23211TT4339</t>
+  </si>
+  <si>
+    <t>21211TT4361</t>
+  </si>
+  <si>
+    <t>23211TT4749</t>
+  </si>
+  <si>
+    <t>23211TT0610</t>
+  </si>
+  <si>
+    <t>23211TT3247</t>
+  </si>
+  <si>
+    <t>23211TT1174</t>
+  </si>
+  <si>
+    <t>22211TT3511</t>
+  </si>
+  <si>
+    <t>23211TT0117</t>
+  </si>
+  <si>
+    <t>23211TT4370</t>
+  </si>
+  <si>
+    <t>22211TT0902</t>
+  </si>
+  <si>
+    <t>22211TT3094</t>
+  </si>
+  <si>
+    <t>23211TT2327</t>
+  </si>
+  <si>
+    <t>23211TT2360</t>
+  </si>
+  <si>
+    <t>23211TT0564</t>
+  </si>
+  <si>
+    <t>22211TT3655</t>
+  </si>
+  <si>
+    <t>22211TT4827</t>
+  </si>
+  <si>
+    <t>23211TT4803</t>
+  </si>
+  <si>
+    <t>NHOM_1</t>
+  </si>
+  <si>
+    <t>NHOM_2</t>
+  </si>
+  <si>
+    <t>NHOM_3</t>
+  </si>
+  <si>
+    <t>NHOM_4</t>
+  </si>
+  <si>
+    <t>NHOM_5</t>
+  </si>
+  <si>
+    <t>NHOM_6</t>
+  </si>
+  <si>
+    <t>NHOM_7</t>
+  </si>
+  <si>
+    <t>NHOM_8</t>
+  </si>
+  <si>
+    <t>NHOM_9</t>
   </si>
 </sst>
 </file>
@@ -133,7 +247,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,7 +262,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -180,12 +336,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D941B3-4561-4CFA-904E-99C092AB619F}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -537,207 +730,647 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="8">
+        <v>2</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="8">
+        <v>2</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="8">
+        <v>2</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="8">
+        <v>2</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="11">
+        <v>3</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="11">
+        <v>3</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="11">
+        <v>3</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="11">
+        <v>3</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="11">
+        <v>3</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="13">
+        <v>4</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="13">
+        <v>4</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="13">
+        <v>4</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="13">
+        <v>4</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="13">
+        <v>4</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="15">
+        <v>5</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="15">
+        <v>5</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="15">
+        <v>5</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="15">
+        <v>5</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="15">
+        <v>5</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="17">
+        <v>6</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="17">
+        <v>6</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="17">
+        <v>6</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="17">
+        <v>6</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="17">
+        <v>6</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="19">
         <v>7</v>
       </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="D32" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="19">
+        <v>7</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="19">
+        <v>7</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="19">
+        <v>7</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="19">
+        <v>7</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="21">
         <v>8</v>
       </c>
-      <c r="C3" s="4">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="D37" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="21">
+        <v>8</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="21">
+        <v>8</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="21">
+        <v>8</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="21">
+        <v>8</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="4">
         <v>9</v>
       </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="D42" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="4">
         <v>9</v>
       </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="D43" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="4">
+        <v>9</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="4">
+        <v>9</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3">
-        <v>3</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="4">
         <v>9</v>
       </c>
-      <c r="C9" s="3">
-        <v>3</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="3">
-        <v>3</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="3">
-        <v>4</v>
-      </c>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="3">
-        <v>4</v>
-      </c>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="3">
-        <v>5</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="3">
-        <v>5</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="3">
-        <v>5</v>
-      </c>
-      <c r="D15" s="3"/>
+      <c r="D46" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>